<commit_message>
Upload a clear excel form
</commit_message>
<xml_diff>
--- a/public/documents/business-process-health-assessment.xlsx
+++ b/public/documents/business-process-health-assessment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimlo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimlo\Desktop\Projects\lowrys-website\public\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904AABE8-1F5C-4A1F-815D-8B3903F93A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE44FF0-7980-4797-BCC9-B336B83F8221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="171">
   <si>
     <t>BUSINESS PROCESS HEALTH ASSESSMENT TOOL</t>
   </si>
@@ -551,19 +551,17 @@
   </si>
   <si>
     <t>For additional assistance, contact:</t>
-  </si>
-  <si>
-    <t>Airtisan.net</t>
-  </si>
-  <si>
-    <t>AI Tech</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +618,13 @@
       <i/>
       <sz val="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -684,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -692,11 +697,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -716,31 +814,53 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="5" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -842,25 +962,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1256,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1386,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="18"/>
@@ -1280,7 +1400,7 @@
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="18"/>
@@ -1294,7 +1414,7 @@
       <c r="J2" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="18"/>
@@ -1324,7 +1444,7 @@
       <c r="J6" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="18"/>
@@ -1408,7 +1528,7 @@
       <c r="J14" s="18"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="18"/>
@@ -1422,7 +1542,7 @@
       <c r="J17" s="18"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="18"/>
@@ -1439,7 +1559,7 @@
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="18"/>
@@ -1468,7 +1588,7 @@
       <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="18"/>
@@ -1482,7 +1602,7 @@
       <c r="J23" s="18"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="18"/>
@@ -1538,7 +1658,7 @@
       <c r="J29" s="18"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="18"/>
@@ -1553,6 +1673,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A29:J29"/>
     <mergeCell ref="A31:J31"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="A11:J11"/>
@@ -1569,10 +1693,6 @@
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A29:J29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1582,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1716,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="18"/>
@@ -1605,7 +1725,7 @@
       <c r="E1" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="18"/>
@@ -1617,59 +1737,49 @@
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="18">
-        <v>1</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="18">
-        <v>100000</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="33">
-        <v>45810</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="18"/>
@@ -1678,7 +1788,7 @@
       <c r="E12" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="18"/>
@@ -1687,7 +1797,7 @@
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="18"/>
@@ -1789,7 +1899,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="18"/>
@@ -1817,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,12 +1938,13 @@
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="80.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="7" width="5" customWidth="1"/>
+    <col min="4" max="4" width="2" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
+    <col min="6" max="8" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="18"/>
@@ -1842,8 +1953,9 @@
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>43</v>
       </c>
@@ -1853,9 +1965,10 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="18"/>
@@ -1864,8 +1977,9 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="18"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -1875,341 +1989,342 @@
       <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="38"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="38"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>50</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="39"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="39"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="39"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="38"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="38"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" t="s">
         <v>55</v>
       </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="38"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="38"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" t="s">
         <v>60</v>
       </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" t="s">
         <v>61</v>
       </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="39"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="39"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" t="s">
         <v>63</v>
       </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="39"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
       </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="38"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="38"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="39"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" t="s">
         <v>66</v>
       </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="39"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="39"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" t="s">
         <v>68</v>
       </c>
-      <c r="C28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="39"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="39"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B30" t="s">
         <v>69</v>
       </c>
-      <c r="C30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="38"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="39"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="39"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" t="s">
         <v>71</v>
       </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="39"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="C33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="39"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="39"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="39"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
         <v>74</v>
       </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="38"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="38"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" t="s">
         <v>75</v>
       </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="39"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" t="s">
         <v>76</v>
       </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="39"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" t="s">
         <v>77</v>
       </c>
-      <c r="C39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="39"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" t="s">
         <v>78</v>
       </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="39"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>79</v>
       </c>
-      <c r="C42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="38"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="38"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" t="s">
         <v>80</v>
       </c>
-      <c r="C43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="39"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="39"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="39"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" t="s">
         <v>82</v>
       </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="39"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="39"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" t="s">
         <v>83</v>
       </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="21" t="s">
+      <c r="C46" s="39"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="39"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="18"/>
@@ -2218,16 +2333,17 @@
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" sqref="C42:C46 C36:C40 C30:C34 C24:C28 C18:C22 C12:C16 C6:C10" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="whole" sqref="C36:E40 C30:E34 C24:E28 C18:E22 C12:E16 C6:E10 C42:E46" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>1</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -2240,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2369,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>84</v>
       </c>
       <c r="B1" s="18"/>
@@ -2266,13 +2382,13 @@
       <c r="I1" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>85</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="22" t="s">
         <v>86</v>
       </c>
       <c r="H3" s="18"/>
@@ -2283,8 +2399,8 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <f>ROUND(SUMPRODUCT(B8:B14,C8:C14)/100,1)</f>
-        <v>4</v>
+        <f>IFERROR(ROUND(SUMPRODUCT(B8:B14,C8:C14)/100,1),"")</f>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>88</v>
@@ -2295,8 +2411,8 @@
         <v>89</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(B4&lt;4,"Poor",IF(B4&lt;7,"Fair",IF(B4&lt;9,"Good","Excellent")))</f>
-        <v>Fair</v>
+        <f>IF(B4="","",IF(B4&lt;4,"Poor",IF(B4&lt;7,"Fair",IF(B4&lt;9,"Good","Excellent"))))</f>
+        <v>Poor</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2320,151 +2436,151 @@
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8">
-        <f>ROUND(AVERAGE(Assessment!C6:C10),1)</f>
-        <v>5</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="41" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C6:C10),1),"")</f>
+        <v/>
+      </c>
+      <c r="C8" s="42">
         <f>'Company Profile'!B17</f>
         <v>14.29</v>
       </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D14" si="0">ROUND(B8*C8/100,2)</f>
-        <v>0.71</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" ref="E8:E14" si="1">IF(B8&lt;4,"Poor",IF(B8&lt;7,"Fair",IF(B8&lt;9,"Good","Excellent")))</f>
-        <v>Fair</v>
+      <c r="D8" s="42" t="str">
+        <f>IFERROR(ROUND(B8*C8/100,2),"")</f>
+        <v/>
+      </c>
+      <c r="E8" s="42" t="str">
+        <f>IF(B8="","",IFERROR(IF(B8&lt;4,"Poor",IF(B8&lt;7,"Fair",IF(B8&lt;9,"Good","Excellent"))),""))</f>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9">
-        <f>ROUND(AVERAGE(Assessment!C11:C15),1)</f>
-        <v>4</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="43" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C11:C15),1),"")</f>
+        <v/>
+      </c>
+      <c r="C9" s="44">
         <f>'Company Profile'!B18</f>
         <v>14.29</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v>Fair</v>
+      <c r="D9" s="44" t="str">
+        <f>IFERROR(ROUND(B9*C9/100,2),"")</f>
+        <v/>
+      </c>
+      <c r="E9" s="44" t="str">
+        <f>IF(B9="","",IFERROR(IF(B9&lt;4,"Poor",IF(B9&lt;7,"Fair",IF(B9&lt;9,"Good","Excellent"))),""))</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B10">
-        <f>ROUND(AVERAGE(Assessment!C16:C20),1)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="43" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C8:C12),1),"")</f>
+        <v/>
+      </c>
+      <c r="C10" s="44">
         <f>'Company Profile'!B19</f>
         <v>14.29</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v>Poor</v>
+      <c r="D10" s="44" t="str">
+        <f t="shared" ref="D10:D14" si="0">IFERROR(ROUND(B10*C10/100,2),"")</f>
+        <v/>
+      </c>
+      <c r="E10" s="44" t="str">
+        <f t="shared" ref="E10:E14" si="1">IF(B10="","",IFERROR(IF(B10&lt;4,"Poor",IF(B10&lt;7,"Fair",IF(B10&lt;9,"Good","Excellent"))),""))</f>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B11">
-        <f>ROUND(AVERAGE(Assessment!C21:C25),1)</f>
-        <v>3.5</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="43" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C13:C17),1),"")</f>
+        <v/>
+      </c>
+      <c r="C11" s="44">
         <f>'Company Profile'!B20</f>
         <v>14.29</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="E11" t="str">
+        <v/>
+      </c>
+      <c r="E11" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>Poor</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B12">
-        <f>ROUND(AVERAGE(Assessment!C26:C30),1)</f>
-        <v>4.5</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="43" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C10:C14),1),"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="44">
         <f>'Company Profile'!B21</f>
         <v>14.29</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>0.64</v>
-      </c>
-      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="E12" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>Fair</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B13">
-        <f>ROUND(AVERAGE(Assessment!C31:C35),1)</f>
-        <v>4</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="43" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C15:C19),1),"")</f>
+        <v/>
+      </c>
+      <c r="C13" s="44">
         <f>'Company Profile'!B22</f>
         <v>14.29</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="E13" t="str">
+        <v/>
+      </c>
+      <c r="E13" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>Fair</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B14">
-        <f>ROUND(AVERAGE(Assessment!C36:C40),1)</f>
-        <v>3.2</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="43" t="str">
+        <f>IFERROR(ROUND(AVERAGE(Assessment!C12:C16),1),"")</f>
+        <v/>
+      </c>
+      <c r="C14" s="44">
         <f>'Company Profile'!B23</f>
         <v>14.29</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="44" t="str">
         <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="E14" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>Poor</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>94</v>
       </c>
       <c r="B16" s="18"/>
@@ -2490,161 +2606,161 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f>RANK(E19,E19:E25)</f>
-        <v>7</v>
-      </c>
-      <c r="B19" t="str">
+      <c r="A19" s="38" t="str">
+        <f>IF(E19="","",RANK(E19,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B19" s="41" t="str">
         <f t="shared" ref="B19:C25" si="2">A8</f>
         <v>Financial Process Efficiency</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <f t="shared" ref="D19:D25" si="3">10-C19</f>
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <f t="shared" ref="E19:E25" si="4">D19*C8/100</f>
-        <v>0.71449999999999991</v>
+      <c r="C19" s="41" t="str">
+        <f>B8</f>
+        <v/>
+      </c>
+      <c r="D19" s="42" t="str">
+        <f>IFERROR(10-C19,"")</f>
+        <v/>
+      </c>
+      <c r="E19" s="42" t="str">
+        <f>IF(D19="","",D19*C8/100)</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f>RANK(E20,E19:E25)</f>
-        <v>4</v>
-      </c>
-      <c r="B20" t="str">
+      <c r="A20" s="39" t="str">
+        <f>IF(E20="","",RANK(E20,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B20" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Operational Workflow</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="43" t="str">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="4"/>
-        <v>0.85739999999999994</v>
+        <v/>
+      </c>
+      <c r="D20" s="44" t="str">
+        <f>IFERROR(10-C20,"")</f>
+        <v/>
+      </c>
+      <c r="E20" s="44" t="str">
+        <f>IF(D20="","",D20*C9/100)</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f>RANK(E21,E19:E25)</f>
-        <v>2</v>
-      </c>
-      <c r="B21" t="str">
+      <c r="A21" s="39" t="str">
+        <f>IF(E21="","",RANK(E21,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B21" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Information Flow &amp; Reporting</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="43" t="str">
         <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="3"/>
-        <v>6.5</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="4"/>
-        <v>0.92884999999999995</v>
+        <v/>
+      </c>
+      <c r="D21" s="44" t="str">
+        <f t="shared" ref="D21:D25" si="3">IFERROR(10-C21,"")</f>
+        <v/>
+      </c>
+      <c r="E21" s="44" t="str">
+        <f t="shared" ref="E21:E25" si="4">IF(D21="","",D21*C10/100)</f>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f>RANK(E22,E19:E25)</f>
-        <v>2</v>
-      </c>
-      <c r="B22" t="str">
+      <c r="A22" s="39" t="str">
+        <f>IF(E22="","",RANK(E22,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B22" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Decision-Making Processes</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="43" t="str">
         <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="D22">
+        <v/>
+      </c>
+      <c r="D22" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>6.5</v>
-      </c>
-      <c r="E22">
+        <v/>
+      </c>
+      <c r="E22" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>0.92884999999999995</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f>RANK(E23,E19:E25)</f>
-        <v>6</v>
-      </c>
-      <c r="B23" t="str">
+      <c r="A23" s="39" t="str">
+        <f>IF(E23="","",RANK(E23,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B23" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Resource Allocation</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="43" t="str">
         <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="D23">
+        <v/>
+      </c>
+      <c r="D23" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-      <c r="E23">
+        <v/>
+      </c>
+      <c r="E23" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>0.78595000000000004</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f>RANK(E24,E19:E25)</f>
-        <v>4</v>
-      </c>
-      <c r="B24" t="str">
+      <c r="A24" s="39" t="str">
+        <f>IF(E24="","",RANK(E24,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B24" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Technology Integration</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="43" t="str">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="D24">
+        <v/>
+      </c>
+      <c r="D24" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="E24">
+        <v/>
+      </c>
+      <c r="E24" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>0.85739999999999994</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f>RANK(E25,E19:E25)</f>
-        <v>1</v>
-      </c>
-      <c r="B25" t="str">
+      <c r="A25" s="39" t="str">
+        <f>IF(E25="","",RANK(E25,E19:E25))</f>
+        <v/>
+      </c>
+      <c r="B25" s="43" t="str">
         <f t="shared" si="2"/>
         <v>Process Documentation</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="43" t="str">
         <f t="shared" si="2"/>
-        <v>3.2</v>
-      </c>
-      <c r="D25">
+        <v/>
+      </c>
+      <c r="D25" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>6.8</v>
-      </c>
-      <c r="E25">
+        <v/>
+      </c>
+      <c r="E25" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>0.97171999999999992</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="18"/>
@@ -2673,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:F9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2687,7 +2803,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="18"/>
@@ -2697,7 +2813,7 @@
       <c r="F1" s="18"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="23" t="s">
         <v>100</v>
       </c>
       <c r="B3" s="18"/>
@@ -2707,7 +2823,7 @@
       <c r="F3" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="18"/>
@@ -2731,17 +2847,17 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="38" t="str">
         <f>'Results Dashboard'!A19</f>
-        <v>7</v>
+        <v/>
       </c>
       <c r="B8" t="str">
         <f>'Results Dashboard'!B19</f>
         <v>Financial Process Efficiency</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="38" t="str">
         <f>'Results Dashboard'!C19</f>
-        <v>5</v>
+        <v/>
       </c>
       <c r="D8" s="18" t="s">
         <v>103</v>
@@ -2750,17 +2866,17 @@
       <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="39" t="str">
         <f>'Results Dashboard'!A20</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="B9" t="str">
         <f>'Results Dashboard'!B20</f>
         <v>Operational Workflow</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="39" t="str">
         <f>'Results Dashboard'!C20</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="D9" s="18" t="s">
         <v>103</v>
@@ -2769,17 +2885,17 @@
       <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="39" t="str">
         <f>'Results Dashboard'!A21</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="B10" t="str">
         <f>'Results Dashboard'!B21</f>
         <v>Information Flow &amp; Reporting</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="39" t="str">
         <f>'Results Dashboard'!C21</f>
-        <v>3.5</v>
+        <v/>
       </c>
       <c r="D10" s="18" t="s">
         <v>103</v>
@@ -2788,7 +2904,7 @@
       <c r="F10" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B12" s="18"/>
@@ -2798,7 +2914,7 @@
       <c r="F12" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="18"/>
@@ -2838,7 +2954,7 @@
       <c r="F17" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="26" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="18"/>
@@ -2878,7 +2994,7 @@
       <c r="F22" s="18"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="30" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="18"/>
@@ -2918,7 +3034,7 @@
       <c r="F27" s="18"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="31" t="s">
         <v>37</v>
       </c>
       <c r="B29" s="18"/>
@@ -2958,7 +3074,7 @@
       <c r="F32" s="18"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="28" t="s">
         <v>38</v>
       </c>
       <c r="B34" s="18"/>
@@ -2998,7 +3114,7 @@
       <c r="F37" s="18"/>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="29" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="18"/>
@@ -3049,7 +3165,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="27" t="s">
         <v>40</v>
       </c>
       <c r="B44" s="18"/>
@@ -3111,7 +3227,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="22" t="s">
         <v>131</v>
       </c>
       <c r="B50" s="18"/>
@@ -3204,7 +3320,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+      <c r="A59" s="23" t="s">
         <v>140</v>
       </c>
       <c r="B59" s="18"/>
@@ -3225,7 +3341,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="20" t="s">
         <v>142</v>
       </c>
       <c r="B61" s="18"/>
@@ -3255,7 +3371,7 @@
       <c r="F63" s="18"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B65" s="18"/>
@@ -3266,12 +3382,20 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A42:F42"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A16:F16"/>
     <mergeCell ref="A65:F65"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A44:F44"/>
@@ -3285,33 +3409,25 @@
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A62:F62"/>
     <mergeCell ref="A20:F20"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A29:F29"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A50:F50"/>
     <mergeCell ref="A56:F56"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A55:F55"/>
     <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A54:F54"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A27:F27"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3321,7 +3437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3332,7 +3450,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>145</v>
       </c>
       <c r="B1" s="18"/>
@@ -3341,7 +3459,7 @@
       <c r="E1" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>146</v>
       </c>
       <c r="B3" s="18"/>
@@ -3350,7 +3468,7 @@
       <c r="E3" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>147</v>
       </c>
       <c r="B5" s="18"/>
@@ -3368,7 +3486,7 @@
       <c r="E6" s="18"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>149</v>
       </c>
       <c r="B8" s="18"/>
@@ -3386,7 +3504,7 @@
       <c r="E9" s="18"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>151</v>
       </c>
       <c r="B11" s="18"/>
@@ -3404,7 +3522,7 @@
       <c r="E12" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>153</v>
       </c>
       <c r="B14" s="18"/>
@@ -3422,7 +3540,7 @@
       <c r="E15" s="18"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="20" t="s">
         <v>155</v>
       </c>
       <c r="B17" s="18"/>
@@ -3440,7 +3558,7 @@
       <c r="E18" s="18"/>
     </row>
     <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="22" t="s">
         <v>157</v>
       </c>
       <c r="B20" s="18"/>
@@ -3449,7 +3567,7 @@
       <c r="E20" s="18"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="20" t="s">
         <v>158</v>
       </c>
       <c r="B22" s="18"/>
@@ -3460,7 +3578,7 @@
       <c r="E22" s="18"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="20" t="s">
         <v>160</v>
       </c>
       <c r="B24" s="18"/>
@@ -3471,7 +3589,7 @@
       <c r="E24" s="18"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="20" t="s">
         <v>162</v>
       </c>
       <c r="B26" s="18"/>
@@ -3482,7 +3600,7 @@
       <c r="E26" s="18"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="20" t="s">
         <v>164</v>
       </c>
       <c r="B28" s="18"/>
@@ -3493,7 +3611,7 @@
       <c r="E28" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="22" t="s">
         <v>166</v>
       </c>
       <c r="B32" s="18"/>
@@ -3529,7 +3647,7 @@
       <c r="E36" s="18"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="23" t="s">
         <v>170</v>
       </c>
       <c r="B40" s="18"/>
@@ -3538,7 +3656,7 @@
       <c r="E40" s="18"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="20" t="s">
         <v>142</v>
       </c>
       <c r="B42" s="18"/>
@@ -3565,7 +3683,7 @@
       <c r="E44" s="18"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B46" s="18"/>
@@ -3575,14 +3693,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C26:E26"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A6:E6"/>
@@ -3599,6 +3709,14 @@
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A15:E15"/>

</xml_diff>